<commit_message>
Update bab 3 One Hot Encoding
</commit_message>
<xml_diff>
--- a/Datasets/Perhitungan.xlsx
+++ b/Datasets/Perhitungan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROG\Documents\skripsi\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B87C5-BF71-4FC9-99B4-BF7021FA6315}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50372A85-332F-407A-B77F-50973B59D20D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3731" windowWidth="18851" windowHeight="9962" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -451,53 +451,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N304"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -13835,6 +13835,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18424,7 +18425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AFEAD8-9121-4498-B9F3-952B280AF1C5}">
   <dimension ref="A1:D304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+    <sheetView topLeftCell="A274" workbookViewId="0">
       <selection activeCell="E294" sqref="E294"/>
     </sheetView>
   </sheetViews>

</xml_diff>